<commit_message>
pandas merge sheet name
</commit_message>
<xml_diff>
--- a/class_info.xlsx
+++ b/class_info.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\kyle\code\python\python_basic\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54BC58CF-FB41-49C6-8327-5EFCAFD29237}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A44B4F0-968F-4AB1-8DE4-A845AF4F73BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11115" yWindow="135" windowWidth="17685" windowHeight="15345" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="class1" sheetId="1" r:id="rId1"/>
+    <sheet name="class2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="31">
   <si>
     <t>姓名</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -116,6 +117,38 @@
   </si>
   <si>
     <t>學生, 班長</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>monkey</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>lion</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>fish</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>bird</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>liopard</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>rabbit</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>mouse</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>額外的欄位</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -443,8 +476,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -566,4 +599,157 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95DF9DB7-4F73-44EB-8A7E-D8581130774B}">
+  <dimension ref="A1:E8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>601</v>
+      </c>
+      <c r="B2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>601</v>
+      </c>
+      <c r="B3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>601</v>
+      </c>
+      <c r="B4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>602</v>
+      </c>
+      <c r="B5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>602</v>
+      </c>
+      <c r="B6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>602</v>
+      </c>
+      <c r="B7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>603</v>
+      </c>
+      <c r="B8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" t="s">
+        <v>19</v>
+      </c>
+      <c r="E8">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>